<commit_message>
Grad reserach seminar loose conflict addition
</commit_message>
<xml_diff>
--- a/course_schedule_results.xlsx
+++ b/course_schedule_results.xlsx
@@ -470,11 +470,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>711</v>
+        <v>332</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probability &amp; Measure </t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -482,7 +482,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -493,11 +493,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>199</v>
+        <v>325</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -539,11 +539,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>610</v>
+        <v>521</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -562,11 +562,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>323</v>
+        <v>101</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -585,11 +585,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -608,19 +608,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>701</v>
+        <v>322</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Graduate Research Seminar</t>
+          <t>Study design</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -631,11 +631,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>240</v>
+        <v>542</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t xml:space="preserve">Intro Time Series  </t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -643,7 +643,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -700,11 +700,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>322</v>
+        <v>199</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Study design</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -723,11 +723,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>332</v>
+        <v>532</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -735,7 +735,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -746,11 +746,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>440</v>
+        <v>610</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -758,7 +758,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -769,11 +769,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>325</v>
+        <v>721</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -792,11 +792,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>402</v>
+        <v>440</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -815,11 +815,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>198</v>
+        <v>402</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -838,11 +838,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>571</v>
+        <v>240</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -850,7 +850,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -884,11 +884,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>523</v>
+        <v>571</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -907,11 +907,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>521</v>
+        <v>323</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -953,11 +953,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>101</v>
+        <v>198</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -976,11 +976,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>721</v>
+        <v>711</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t xml:space="preserve">Probability &amp; Measure </t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1045,15 +1045,15 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>542</v>
+        <v>701</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intro Time Series  </t>
+          <t>Graduate Research Seminar</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1112,16 +1112,16 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1135,11 +1135,11 @@
         <v>110</v>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1158,16 +1158,16 @@
         <v>198</v>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1227,11 +1227,11 @@
         <v>240</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1250,7 +1250,7 @@
         <v>322</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1273,16 +1273,16 @@
         <v>323</v>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1296,16 +1296,16 @@
         <v>325</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1319,16 +1319,16 @@
         <v>332</v>
       </c>
       <c r="B11" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1342,11 +1342,11 @@
         <v>402</v>
       </c>
       <c r="B12" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1365,16 +1365,16 @@
         <v>410</v>
       </c>
       <c r="B13" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1388,16 +1388,16 @@
         <v>440</v>
       </c>
       <c r="B14" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1411,16 +1411,16 @@
         <v>521</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1434,16 +1434,16 @@
         <v>522</v>
       </c>
       <c r="B16" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1457,16 +1457,16 @@
         <v>523</v>
       </c>
       <c r="B17" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1480,11 +1480,11 @@
         <v>532</v>
       </c>
       <c r="B18" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1503,16 +1503,16 @@
         <v>542</v>
       </c>
       <c r="B19" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1526,16 +1526,16 @@
         <v>571</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1549,16 +1549,16 @@
         <v>581</v>
       </c>
       <c r="B21" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1572,11 +1572,11 @@
         <v>602</v>
       </c>
       <c r="B22" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1595,11 +1595,11 @@
         <v>610</v>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1618,16 +1618,16 @@
         <v>701</v>
       </c>
       <c r="B24" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1641,11 +1641,11 @@
         <v>702</v>
       </c>
       <c r="B25" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1664,16 +1664,16 @@
         <v>711</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1687,16 +1687,16 @@
         <v>721</v>
       </c>
       <c r="B27" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1773,11 +1773,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>711</v>
+        <v>332</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probability &amp; Measure </t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1785,20 +1785,20 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -1809,11 +1809,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>199</v>
+        <v>325</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1825,11 +1825,11 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -1861,11 +1861,11 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -1881,11 +1881,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>610</v>
+        <v>521</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1897,16 +1897,16 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -1917,11 +1917,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>323</v>
+        <v>101</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1933,16 +1933,16 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -1953,11 +1953,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1969,11 +1969,11 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1989,32 +1989,32 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>701</v>
+        <v>322</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Graduate Research Seminar</t>
+          <t>Study design</t>
         </is>
       </c>
       <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Ugrad</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Grad</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>7</v>
-      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2025,11 +2025,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>240</v>
+        <v>542</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t xml:space="preserve">Intro Time Series  </t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2037,15 +2037,15 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -2113,16 +2113,16 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2133,11 +2133,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>322</v>
+        <v>199</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Study design</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -2169,11 +2169,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>332</v>
+        <v>532</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -2181,20 +2181,20 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2205,11 +2205,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>440</v>
+        <v>610</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -2217,20 +2217,20 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2241,11 +2241,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>325</v>
+        <v>721</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -2253,20 +2253,20 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2277,11 +2277,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>402</v>
+        <v>440</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -2293,16 +2293,16 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2313,11 +2313,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>198</v>
+        <v>402</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -2349,11 +2349,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>571</v>
+        <v>240</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -2361,15 +2361,15 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -2401,11 +2401,11 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -2421,11 +2421,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>523</v>
+        <v>571</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -2437,11 +2437,11 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -2457,11 +2457,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>521</v>
+        <v>323</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -2469,20 +2469,20 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2509,16 +2509,16 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2529,11 +2529,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>101</v>
+        <v>198</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -2565,11 +2565,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>721</v>
+        <v>711</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t xml:space="preserve">Probability &amp; Measure </t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -2581,11 +2581,11 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2617,11 +2617,11 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2653,16 +2653,16 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2673,15 +2673,15 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>542</v>
+        <v>701</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intro Time Series  </t>
+          <t>Graduate Research Seminar</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -2689,7 +2689,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -2698,7 +2698,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2760,24 +2760,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>199</v>
+        <v>325</v>
       </c>
       <c r="C2" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2791,7 +2791,7 @@
         <v>602</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -2800,7 +2800,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2816,24 +2816,24 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>610</v>
+        <v>521</v>
       </c>
       <c r="C4" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2844,19 +2844,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>323</v>
+        <v>101</v>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2868,23 +2868,23 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>240</v>
+        <v>523</v>
       </c>
       <c r="C6" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2903,7 +2903,7 @@
         <v>221</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2931,7 +2931,7 @@
         <v>410</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -2940,147 +2940,147 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>I</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>440</v>
+        <v>199</v>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>K</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>325</v>
+        <v>610</v>
       </c>
       <c r="C10" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>402</v>
+        <v>721</v>
       </c>
       <c r="C11" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>198</v>
+        <v>440</v>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>702</v>
+        <v>402</v>
       </c>
       <c r="C13" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -3092,23 +3092,23 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>O</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>523</v>
+        <v>240</v>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -3120,18 +3120,18 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>521</v>
+        <v>702</v>
       </c>
       <c r="C15" t="n">
         <v>15</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -3148,23 +3148,23 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>R</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>101</v>
+        <v>323</v>
       </c>
       <c r="C16" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -3176,18 +3176,18 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>721</v>
+        <v>198</v>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added loose conflict that all 500 and 600 level classes should not overlap, and labs of assoc. classes.
</commit_message>
<xml_diff>
--- a/course_schedule_results.xlsx
+++ b/course_schedule_results.xlsx
@@ -470,11 +470,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>332</v>
+        <v>610</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -482,7 +482,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -493,11 +493,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>325</v>
+        <v>523</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -505,7 +505,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -516,11 +516,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>602</v>
+        <v>221</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -528,7 +528,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -562,11 +562,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>101</v>
+        <v>198</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -585,11 +585,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>523</v>
+        <v>323</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -597,7 +597,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -608,11 +608,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>322</v>
+        <v>522</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Study design</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -631,11 +631,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>542</v>
+        <v>322</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intro Time Series  </t>
+          <t>Study design</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -643,7 +643,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -654,11 +654,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>221</v>
+        <v>410</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -677,11 +677,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>410</v>
+        <v>440</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -700,11 +700,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -723,11 +723,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>532</v>
+        <v>602</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -746,11 +746,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>610</v>
+        <v>721</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -769,11 +769,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>721</v>
+        <v>325</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -792,11 +792,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>440</v>
+        <v>402</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -815,11 +815,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>402</v>
+        <v>542</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t xml:space="preserve">Intro Time Series  </t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -827,7 +827,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -838,11 +838,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>240</v>
+        <v>711</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t xml:space="preserve">Probability &amp; Measure </t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -850,7 +850,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -861,11 +861,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>702</v>
+        <v>199</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -873,7 +873,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -907,11 +907,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>323</v>
+        <v>532</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -953,11 +953,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>198</v>
+        <v>101</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -976,11 +976,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>711</v>
+        <v>332</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probability &amp; Measure </t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -1022,11 +1022,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>522</v>
+        <v>702</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1112,16 +1112,16 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1135,7 +1135,7 @@
         <v>110</v>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1181,16 +1181,16 @@
         <v>199</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1204,16 +1204,16 @@
         <v>221</v>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1227,16 +1227,16 @@
         <v>240</v>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1250,16 +1250,16 @@
         <v>322</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1273,16 +1273,16 @@
         <v>323</v>
       </c>
       <c r="B9" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1296,16 +1296,16 @@
         <v>325</v>
       </c>
       <c r="B10" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1319,16 +1319,16 @@
         <v>332</v>
       </c>
       <c r="B11" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1342,16 +1342,16 @@
         <v>402</v>
       </c>
       <c r="B12" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1365,16 +1365,16 @@
         <v>410</v>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1388,16 +1388,16 @@
         <v>440</v>
       </c>
       <c r="B14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1411,7 +1411,7 @@
         <v>521</v>
       </c>
       <c r="B15" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1434,11 +1434,11 @@
         <v>522</v>
       </c>
       <c r="B16" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1457,16 +1457,16 @@
         <v>523</v>
       </c>
       <c r="B17" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1480,16 +1480,16 @@
         <v>532</v>
       </c>
       <c r="B18" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1503,16 +1503,16 @@
         <v>542</v>
       </c>
       <c r="B19" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1526,16 +1526,16 @@
         <v>571</v>
       </c>
       <c r="B20" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1549,16 +1549,16 @@
         <v>581</v>
       </c>
       <c r="B21" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1572,16 +1572,16 @@
         <v>602</v>
       </c>
       <c r="B22" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1595,11 +1595,11 @@
         <v>610</v>
       </c>
       <c r="B23" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1641,16 +1641,16 @@
         <v>702</v>
       </c>
       <c r="B25" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1664,16 +1664,16 @@
         <v>711</v>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1687,7 +1687,7 @@
         <v>721</v>
       </c>
       <c r="B27" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1773,11 +1773,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>332</v>
+        <v>610</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1785,11 +1785,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -1809,11 +1809,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>325</v>
+        <v>523</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1821,11 +1821,11 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -1845,11 +1845,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>602</v>
+        <v>221</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1857,20 +1857,20 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -1917,11 +1917,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>101</v>
+        <v>198</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1933,16 +1933,16 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -1953,11 +1953,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>523</v>
+        <v>323</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -1989,11 +1989,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>322</v>
+        <v>522</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Study design</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -2001,20 +2001,20 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2025,11 +2025,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>542</v>
+        <v>322</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intro Time Series  </t>
+          <t>Study design</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2037,15 +2037,15 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -2061,11 +2061,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>221</v>
+        <v>410</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -2077,11 +2077,11 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -2097,11 +2097,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>410</v>
+        <v>440</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -2113,7 +2113,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2133,11 +2133,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -2149,16 +2149,16 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2169,11 +2169,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>532</v>
+        <v>602</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -2205,11 +2205,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>610</v>
+        <v>721</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -2221,11 +2221,11 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -2241,11 +2241,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>721</v>
+        <v>325</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -2253,15 +2253,15 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -2277,11 +2277,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>440</v>
+        <v>402</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -2293,11 +2293,11 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -2313,11 +2313,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>402</v>
+        <v>542</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t xml:space="preserve">Intro Time Series  </t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -2325,20 +2325,20 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2349,11 +2349,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>240</v>
+        <v>711</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t xml:space="preserve">Probability &amp; Measure </t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -2361,11 +2361,11 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -2374,7 +2374,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2385,11 +2385,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>702</v>
+        <v>199</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -2437,16 +2437,16 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2457,11 +2457,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>323</v>
+        <v>532</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -2469,15 +2469,15 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -2509,16 +2509,16 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2529,11 +2529,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>198</v>
+        <v>101</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -2545,16 +2545,16 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2565,11 +2565,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>711</v>
+        <v>332</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probability &amp; Measure </t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -2577,15 +2577,15 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2617,7 +2617,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2637,11 +2637,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>522</v>
+        <v>702</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -2653,16 +2653,16 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2756,23 +2756,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>325</v>
+        <v>610</v>
       </c>
       <c r="C2" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2784,84 +2784,84 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>602</v>
+        <v>523</v>
       </c>
       <c r="C3" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>521</v>
+        <v>221</v>
       </c>
       <c r="C4" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>521</v>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2872,19 +2872,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>523</v>
+        <v>198</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2896,23 +2896,23 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>221</v>
+        <v>323</v>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2931,7 +2931,7 @@
         <v>410</v>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -2940,63 +2940,63 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>199</v>
+        <v>440</v>
       </c>
       <c r="C9" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>I</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>610</v>
+        <v>240</v>
       </c>
       <c r="C10" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -3008,51 +3008,51 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>J</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>721</v>
+        <v>602</v>
       </c>
       <c r="C11" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>K</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>440</v>
+        <v>721</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -3064,51 +3064,51 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>402</v>
+        <v>325</v>
       </c>
       <c r="C13" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>M</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>240</v>
+        <v>402</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -3124,75 +3124,75 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>702</v>
+        <v>199</v>
       </c>
       <c r="C15" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>T</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>323</v>
+        <v>101</v>
       </c>
       <c r="C16" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>198</v>
+        <v>702</v>
       </c>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">

</xml_diff>

<commit_message>
Prime time conflict addition
</commit_message>
<xml_diff>
--- a/course_schedule_results.xlsx
+++ b/course_schedule_results.xlsx
@@ -470,11 +470,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>610</v>
+        <v>702</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -493,11 +493,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -516,11 +516,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>221</v>
+        <v>602</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -528,7 +528,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -539,11 +539,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>521</v>
+        <v>571</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -585,11 +585,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>323</v>
+        <v>523</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -597,7 +597,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -608,11 +608,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>522</v>
+        <v>199</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -631,11 +631,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>322</v>
+        <v>110</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Study design</t>
+          <t xml:space="preserve">Focus </t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -700,11 +700,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>240</v>
+        <v>522</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -712,7 +712,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -723,11 +723,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>602</v>
+        <v>240</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -735,7 +735,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -746,11 +746,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>721</v>
+        <v>610</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -769,11 +769,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>325</v>
+        <v>532</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -792,11 +792,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>402</v>
+        <v>325</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -861,11 +861,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>199</v>
+        <v>322</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Study design</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -884,11 +884,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>571</v>
+        <v>221</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -907,11 +907,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>532</v>
+        <v>323</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -976,11 +976,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>332</v>
+        <v>402</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -999,11 +999,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>110</v>
+        <v>332</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Focus </t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1022,11 +1022,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>702</v>
+        <v>721</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1112,11 +1112,11 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1135,11 +1135,11 @@
         <v>110</v>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1158,16 +1158,16 @@
         <v>198</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1181,16 +1181,16 @@
         <v>199</v>
       </c>
       <c r="B5" t="n">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1204,16 +1204,16 @@
         <v>221</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1227,11 +1227,11 @@
         <v>240</v>
       </c>
       <c r="B7" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1273,16 +1273,16 @@
         <v>323</v>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1296,16 +1296,16 @@
         <v>325</v>
       </c>
       <c r="B10" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1319,11 +1319,11 @@
         <v>332</v>
       </c>
       <c r="B11" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1342,16 +1342,16 @@
         <v>402</v>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1365,16 +1365,16 @@
         <v>410</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1388,16 +1388,16 @@
         <v>440</v>
       </c>
       <c r="B14" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1411,16 +1411,16 @@
         <v>521</v>
       </c>
       <c r="B15" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1434,16 +1434,16 @@
         <v>522</v>
       </c>
       <c r="B16" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1457,11 +1457,11 @@
         <v>523</v>
       </c>
       <c r="B17" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1480,7 +1480,7 @@
         <v>532</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1503,16 +1503,16 @@
         <v>542</v>
       </c>
       <c r="B19" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1526,16 +1526,16 @@
         <v>571</v>
       </c>
       <c r="B20" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1549,16 +1549,16 @@
         <v>581</v>
       </c>
       <c r="B21" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1572,16 +1572,16 @@
         <v>602</v>
       </c>
       <c r="B22" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1595,11 +1595,11 @@
         <v>610</v>
       </c>
       <c r="B23" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1641,16 +1641,16 @@
         <v>702</v>
       </c>
       <c r="B25" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1664,11 +1664,11 @@
         <v>711</v>
       </c>
       <c r="B26" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1687,11 +1687,11 @@
         <v>721</v>
       </c>
       <c r="B27" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1773,11 +1773,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>610</v>
+        <v>702</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1789,11 +1789,11 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -1809,11 +1809,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -1845,11 +1845,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>221</v>
+        <v>602</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1857,20 +1857,20 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -1881,11 +1881,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>521</v>
+        <v>571</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -1933,16 +1933,16 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -1953,11 +1953,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>323</v>
+        <v>523</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1965,11 +1965,11 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -1989,11 +1989,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>522</v>
+        <v>199</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -2001,15 +2001,15 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -2025,11 +2025,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>322</v>
+        <v>110</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Study design</t>
+          <t xml:space="preserve">Focus </t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2041,16 +2041,16 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2077,16 +2077,16 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2113,16 +2113,16 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2133,11 +2133,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>240</v>
+        <v>522</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -2145,20 +2145,20 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2169,11 +2169,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>602</v>
+        <v>240</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -2181,20 +2181,20 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2205,11 +2205,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>721</v>
+        <v>610</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -2221,11 +2221,11 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -2241,11 +2241,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>325</v>
+        <v>532</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -2253,15 +2253,15 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -2277,11 +2277,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>402</v>
+        <v>325</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -2329,16 +2329,16 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2365,11 +2365,11 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -2385,11 +2385,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>199</v>
+        <v>322</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Study design</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -2401,16 +2401,16 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2421,11 +2421,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>571</v>
+        <v>221</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -2457,11 +2457,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>532</v>
+        <v>323</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -2469,11 +2469,11 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2509,16 +2509,16 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2545,11 +2545,11 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2565,11 +2565,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>332</v>
+        <v>402</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -2581,16 +2581,16 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2601,11 +2601,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>110</v>
+        <v>332</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Focus </t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2617,16 +2617,16 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2637,11 +2637,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>702</v>
+        <v>721</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -2653,16 +2653,16 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2760,19 +2760,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>610</v>
+        <v>702</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2788,24 +2788,24 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2816,47 +2816,47 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>221</v>
+        <v>602</v>
       </c>
       <c r="C4" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>521</v>
+        <v>198</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2872,19 +2872,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>198</v>
+        <v>523</v>
       </c>
       <c r="C6" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2896,28 +2896,28 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>323</v>
+        <v>199</v>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2931,7 +2931,7 @@
         <v>410</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2959,7 +2959,7 @@
         <v>440</v>
       </c>
       <c r="C9" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -2968,26 +2968,26 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>J</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>240</v>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -2996,180 +2996,180 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>K</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="C11" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>M</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>721</v>
+        <v>325</v>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>325</v>
+        <v>221</v>
       </c>
       <c r="C13" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>R</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>402</v>
+        <v>323</v>
       </c>
       <c r="C14" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>T</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>199</v>
+        <v>101</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>101</v>
+        <v>402</v>
       </c>
       <c r="C16" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -3180,24 +3180,24 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>702</v>
+        <v>721</v>
       </c>
       <c r="C17" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the 50% constraints for prime times and t/th.
</commit_message>
<xml_diff>
--- a/course_schedule_results.xlsx
+++ b/course_schedule_results.xlsx
@@ -470,11 +470,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>702</v>
+        <v>711</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t xml:space="preserve">Probability &amp; Measure </t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -493,11 +493,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>521</v>
+        <v>323</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -505,7 +505,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -539,11 +539,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>571</v>
+        <v>332</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -551,7 +551,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -562,11 +562,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -585,11 +585,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>523</v>
+        <v>542</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t xml:space="preserve">Intro Time Series  </t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -608,11 +608,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>199</v>
+        <v>521</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -631,11 +631,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Focus </t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -677,11 +677,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>440</v>
+        <v>610</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -689,7 +689,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -700,11 +700,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>522</v>
+        <v>440</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -712,7 +712,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -723,11 +723,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>240</v>
+        <v>402</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -746,11 +746,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>610</v>
+        <v>721</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -815,11 +815,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>542</v>
+        <v>198</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intro Time Series  </t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -827,7 +827,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -838,11 +838,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>711</v>
+        <v>240</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probability &amp; Measure </t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -850,7 +850,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -884,11 +884,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>221</v>
+        <v>571</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -907,11 +907,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>323</v>
+        <v>523</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -953,11 +953,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t xml:space="preserve">Focus </t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -976,11 +976,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>402</v>
+        <v>221</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -999,11 +999,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>332</v>
+        <v>522</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -1022,11 +1022,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>721</v>
+        <v>702</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1112,11 +1112,11 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1135,16 +1135,16 @@
         <v>110</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1158,7 +1158,7 @@
         <v>198</v>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1181,16 +1181,16 @@
         <v>199</v>
       </c>
       <c r="B5" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1204,16 +1204,16 @@
         <v>221</v>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1227,16 +1227,16 @@
         <v>240</v>
       </c>
       <c r="B7" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1250,7 +1250,7 @@
         <v>322</v>
       </c>
       <c r="B8" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1273,16 +1273,16 @@
         <v>323</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1319,16 +1319,16 @@
         <v>332</v>
       </c>
       <c r="B11" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1342,7 +1342,7 @@
         <v>402</v>
       </c>
       <c r="B12" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1365,16 +1365,16 @@
         <v>410</v>
       </c>
       <c r="B13" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1388,16 +1388,16 @@
         <v>440</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1411,7 +1411,7 @@
         <v>521</v>
       </c>
       <c r="B15" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1434,16 +1434,16 @@
         <v>522</v>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1457,16 +1457,16 @@
         <v>523</v>
       </c>
       <c r="B17" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1480,11 +1480,11 @@
         <v>532</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1503,16 +1503,16 @@
         <v>542</v>
       </c>
       <c r="B19" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1526,16 +1526,16 @@
         <v>571</v>
       </c>
       <c r="B20" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1549,16 +1549,16 @@
         <v>581</v>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1572,16 +1572,16 @@
         <v>602</v>
       </c>
       <c r="B22" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1595,7 +1595,7 @@
         <v>610</v>
       </c>
       <c r="B23" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1641,16 +1641,16 @@
         <v>702</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1664,7 +1664,7 @@
         <v>711</v>
       </c>
       <c r="B26" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1687,16 +1687,16 @@
         <v>721</v>
       </c>
       <c r="B27" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1773,11 +1773,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>702</v>
+        <v>711</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t xml:space="preserve">Probability &amp; Measure </t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1789,11 +1789,11 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -1809,11 +1809,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>521</v>
+        <v>323</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -1861,16 +1861,16 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -1881,11 +1881,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>571</v>
+        <v>332</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -1917,11 +1917,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1933,11 +1933,11 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1953,11 +1953,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>523</v>
+        <v>542</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t xml:space="preserve">Intro Time Series  </t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1969,11 +1969,11 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1989,11 +1989,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>199</v>
+        <v>521</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -2025,11 +2025,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Focus </t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2077,16 +2077,16 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2097,11 +2097,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>440</v>
+        <v>610</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -2109,20 +2109,20 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2133,11 +2133,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>522</v>
+        <v>440</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -2145,20 +2145,20 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2169,11 +2169,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>240</v>
+        <v>402</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -2185,7 +2185,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2205,11 +2205,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>610</v>
+        <v>721</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -2221,16 +2221,16 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2257,11 +2257,11 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -2313,11 +2313,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>542</v>
+        <v>198</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intro Time Series  </t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -2325,11 +2325,11 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -2338,7 +2338,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2349,11 +2349,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>711</v>
+        <v>240</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probability &amp; Measure </t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -2361,20 +2361,20 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2401,7 +2401,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2421,11 +2421,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>221</v>
+        <v>571</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -2433,20 +2433,20 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2457,11 +2457,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>323</v>
+        <v>523</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -2469,11 +2469,11 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2509,16 +2509,16 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2529,11 +2529,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t xml:space="preserve">Focus </t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -2545,7 +2545,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -2554,7 +2554,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2565,11 +2565,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>402</v>
+        <v>221</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -2581,16 +2581,16 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2601,11 +2601,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>332</v>
+        <v>522</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2613,20 +2613,20 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2637,11 +2637,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>721</v>
+        <v>702</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -2653,7 +2653,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2756,18 +2756,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>702</v>
+        <v>323</v>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2777,30 +2777,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>521</v>
+        <v>602</v>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2812,18 +2812,18 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>602</v>
+        <v>199</v>
       </c>
       <c r="C4" t="n">
         <v>19</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2840,84 +2840,84 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>198</v>
+        <v>521</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>G</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>523</v>
+        <v>101</v>
       </c>
       <c r="C6" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>H</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>199</v>
+        <v>410</v>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>410</v>
+        <v>610</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -2940,26 +2940,26 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>I</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>440</v>
       </c>
       <c r="C9" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2984,24 +2984,24 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>240</v>
+        <v>402</v>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -3012,24 +3012,24 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>610</v>
+        <v>721</v>
       </c>
       <c r="C11" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -3043,7 +3043,7 @@
         <v>325</v>
       </c>
       <c r="C12" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -3052,30 +3052,30 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="C13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -3085,63 +3085,63 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>O</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>323</v>
+        <v>240</v>
       </c>
       <c r="C14" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>R</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>101</v>
+        <v>523</v>
       </c>
       <c r="C15" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -3152,14 +3152,14 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>402</v>
+        <v>221</v>
       </c>
       <c r="C16" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -3169,7 +3169,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -3180,24 +3180,24 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>721</v>
+        <v>702</v>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
try to fix the conflict
</commit_message>
<xml_diff>
--- a/course_schedule_results.xlsx
+++ b/course_schedule_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Prof_Course_Assignments" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Course_Time_Assignments" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Combined_Schedule" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Lab_Assignments" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Prof_Course_Assignments" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Course_Time_Assignments" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Combined_Schedule" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Lab_Assignments" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -470,11 +470,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>711</v>
+        <v>532</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probability &amp; Measure </t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -493,11 +493,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>323</v>
+        <v>523</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -505,7 +505,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -516,11 +516,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>602</v>
+        <v>702</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -539,11 +539,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>332</v>
+        <v>602</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -551,7 +551,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -562,11 +562,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -585,11 +585,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>542</v>
+        <v>440</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intro Time Series  </t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -597,7 +597,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -631,11 +631,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>101</v>
+        <v>322</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Study design</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -700,11 +700,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>440</v>
+        <v>101</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -723,11 +723,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>402</v>
+        <v>240</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -769,11 +769,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>532</v>
+        <v>325</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -792,11 +792,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>325</v>
+        <v>402</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -815,11 +815,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>198</v>
+        <v>542</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t xml:space="preserve">Intro Time Series  </t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -827,7 +827,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -838,11 +838,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>240</v>
+        <v>571</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -850,7 +850,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -861,11 +861,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>322</v>
+        <v>199</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Study design</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -884,11 +884,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>571</v>
+        <v>323</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -907,11 +907,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>523</v>
+        <v>711</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t xml:space="preserve">Probability &amp; Measure </t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -999,11 +999,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>522</v>
+        <v>332</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -1022,11 +1022,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>702</v>
+        <v>522</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1158,11 +1158,11 @@
         <v>198</v>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1181,16 +1181,16 @@
         <v>199</v>
       </c>
       <c r="B5" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1227,16 +1227,16 @@
         <v>240</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1250,16 +1250,16 @@
         <v>322</v>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1273,16 +1273,16 @@
         <v>323</v>
       </c>
       <c r="B9" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1296,16 +1296,16 @@
         <v>325</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1319,16 +1319,16 @@
         <v>332</v>
       </c>
       <c r="B11" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1342,11 +1342,11 @@
         <v>402</v>
       </c>
       <c r="B12" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1365,16 +1365,16 @@
         <v>410</v>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1388,16 +1388,16 @@
         <v>440</v>
       </c>
       <c r="B14" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1411,11 +1411,11 @@
         <v>521</v>
       </c>
       <c r="B15" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1434,16 +1434,16 @@
         <v>522</v>
       </c>
       <c r="B16" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1457,16 +1457,16 @@
         <v>523</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1480,16 +1480,16 @@
         <v>532</v>
       </c>
       <c r="B18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1503,16 +1503,16 @@
         <v>542</v>
       </c>
       <c r="B19" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1526,11 +1526,11 @@
         <v>571</v>
       </c>
       <c r="B20" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1549,11 +1549,11 @@
         <v>581</v>
       </c>
       <c r="B21" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1572,11 +1572,11 @@
         <v>602</v>
       </c>
       <c r="B22" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1595,16 +1595,16 @@
         <v>610</v>
       </c>
       <c r="B23" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1641,16 +1641,16 @@
         <v>702</v>
       </c>
       <c r="B25" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1664,16 +1664,16 @@
         <v>711</v>
       </c>
       <c r="B26" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1687,16 +1687,16 @@
         <v>721</v>
       </c>
       <c r="B27" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1773,11 +1773,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>711</v>
+        <v>532</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probability &amp; Measure </t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1789,11 +1789,11 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -1809,11 +1809,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>323</v>
+        <v>523</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1821,20 +1821,20 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -1845,11 +1845,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>602</v>
+        <v>702</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1861,11 +1861,11 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -1881,11 +1881,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>332</v>
+        <v>602</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1893,11 +1893,11 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -1917,11 +1917,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -1953,11 +1953,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>542</v>
+        <v>440</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intro Time Series  </t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1965,20 +1965,20 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2005,11 +2005,11 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -2025,11 +2025,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>101</v>
+        <v>322</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Study design</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2041,7 +2041,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2077,16 +2077,16 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2113,16 +2113,16 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2133,11 +2133,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>440</v>
+        <v>101</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -2149,16 +2149,16 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2169,11 +2169,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>402</v>
+        <v>240</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -2185,16 +2185,16 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2221,16 +2221,16 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2241,11 +2241,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>532</v>
+        <v>325</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -2277,11 +2277,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>325</v>
+        <v>402</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -2293,11 +2293,11 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -2313,11 +2313,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>198</v>
+        <v>542</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t xml:space="preserve">Intro Time Series  </t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -2325,11 +2325,11 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -2338,7 +2338,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2349,11 +2349,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>240</v>
+        <v>571</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -2361,20 +2361,20 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2385,11 +2385,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>322</v>
+        <v>199</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Study design</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -2401,7 +2401,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2421,11 +2421,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>571</v>
+        <v>323</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -2433,15 +2433,15 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -2457,11 +2457,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>523</v>
+        <v>711</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t xml:space="preserve">Probability &amp; Measure </t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -2473,7 +2473,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2509,11 +2509,11 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -2601,11 +2601,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>522</v>
+        <v>332</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2613,20 +2613,20 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2637,11 +2637,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>702</v>
+        <v>522</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -2653,16 +2653,16 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2760,24 +2760,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>323</v>
+        <v>523</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Introduction to Programming for StatSci</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2788,19 +2788,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>602</v>
+        <v>702</v>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2812,23 +2812,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>199</v>
+        <v>602</v>
       </c>
       <c r="C4" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2840,23 +2840,23 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>521</v>
+        <v>198</v>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2868,56 +2868,56 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>101</v>
+        <v>440</v>
       </c>
       <c r="C6" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>410</v>
+        <v>521</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>610</v>
+        <v>410</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -2945,25 +2945,25 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>440</v>
+        <v>610</v>
       </c>
       <c r="C9" t="n">
         <v>15</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -2980,79 +2980,79 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>I</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>402</v>
+        <v>101</v>
       </c>
       <c r="C10" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>J</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>721</v>
+        <v>240</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>K</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>325</v>
+        <v>721</v>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -3064,23 +3064,23 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>198</v>
+        <v>325</v>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -3092,23 +3092,23 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>M</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>240</v>
+        <v>402</v>
       </c>
       <c r="C14" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -3120,46 +3120,46 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>523</v>
+        <v>199</v>
       </c>
       <c r="C15" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>221</v>
+        <v>323</v>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Introduction to Programming for StatSci</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -3169,35 +3169,35 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>702</v>
+        <v>221</v>
       </c>
       <c r="C17" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing double booking constraint for professor, and removing redundant one-to-one x,y constraint.
</commit_message>
<xml_diff>
--- a/course_schedule_results.xlsx
+++ b/course_schedule_results.xlsx
@@ -516,11 +516,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>602</v>
+        <v>702</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -539,11 +539,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>332</v>
+        <v>440</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -562,11 +562,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>199</v>
+        <v>523</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -574,7 +574,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -608,11 +608,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>521</v>
+        <v>721</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -631,11 +631,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>101</v>
+        <v>532</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -643,7 +643,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -654,11 +654,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>410</v>
+        <v>221</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -700,11 +700,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>440</v>
+        <v>521</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -712,7 +712,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -723,11 +723,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>402</v>
+        <v>602</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -735,7 +735,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
     </row>
@@ -746,11 +746,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>721</v>
+        <v>410</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -758,7 +758,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -769,11 +769,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>532</v>
+        <v>325</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -792,11 +792,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>325</v>
+        <v>402</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -884,11 +884,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>571</v>
+        <v>199</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -907,11 +907,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>523</v>
+        <v>571</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -953,11 +953,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Focus </t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -976,11 +976,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>221</v>
+        <v>332</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -999,11 +999,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>522</v>
+        <v>110</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t xml:space="preserve">Focus </t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
     </row>
@@ -1022,11 +1022,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>702</v>
+        <v>522</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1112,11 +1112,11 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1135,7 +1135,7 @@
         <v>110</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1158,11 +1158,11 @@
         <v>198</v>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1181,11 +1181,11 @@
         <v>199</v>
       </c>
       <c r="B5" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1204,11 +1204,11 @@
         <v>221</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1227,11 +1227,11 @@
         <v>240</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1250,16 +1250,16 @@
         <v>322</v>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1273,11 +1273,11 @@
         <v>323</v>
       </c>
       <c r="B9" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1296,16 +1296,16 @@
         <v>325</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1319,16 +1319,16 @@
         <v>332</v>
       </c>
       <c r="B11" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1342,16 +1342,16 @@
         <v>402</v>
       </c>
       <c r="B12" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1365,16 +1365,16 @@
         <v>410</v>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1388,16 +1388,16 @@
         <v>440</v>
       </c>
       <c r="B14" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1411,16 +1411,16 @@
         <v>521</v>
       </c>
       <c r="B15" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1434,11 +1434,11 @@
         <v>522</v>
       </c>
       <c r="B16" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1457,16 +1457,16 @@
         <v>523</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1480,16 +1480,16 @@
         <v>532</v>
       </c>
       <c r="B18" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1503,11 +1503,11 @@
         <v>542</v>
       </c>
       <c r="B19" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1526,16 +1526,16 @@
         <v>571</v>
       </c>
       <c r="B20" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1549,11 +1549,11 @@
         <v>581</v>
       </c>
       <c r="B21" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1572,16 +1572,16 @@
         <v>602</v>
       </c>
       <c r="B22" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/F</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1641,11 +1641,11 @@
         <v>702</v>
       </c>
       <c r="B25" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1687,11 +1687,11 @@
         <v>721</v>
       </c>
       <c r="B27" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1825,11 +1825,11 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -1845,11 +1845,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>602</v>
+        <v>702</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1861,16 +1861,16 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -1881,11 +1881,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>332</v>
+        <v>440</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Statistical Inference</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1897,16 +1897,16 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -1917,11 +1917,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>199</v>
+        <v>523</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1929,11 +1929,11 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -1969,11 +1969,11 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1989,11 +1989,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>521</v>
+        <v>721</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -2005,11 +2005,11 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -2025,11 +2025,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>101</v>
+        <v>532</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Theory of Inference</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2037,20 +2037,20 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2061,11 +2061,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>410</v>
+        <v>221</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -2077,16 +2077,16 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2133,11 +2133,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>440</v>
+        <v>521</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -2145,11 +2145,11 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2169,11 +2169,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>402</v>
+        <v>602</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -2181,20 +2181,20 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Ugrad</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2205,11 +2205,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>721</v>
+        <v>410</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -2217,20 +2217,20 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
@@ -2241,11 +2241,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>532</v>
+        <v>325</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Theory of Inference</t>
+          <t>Machine Learning and Data Mining</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -2253,20 +2253,20 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>4:40-5:55pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2277,11 +2277,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>325</v>
+        <v>402</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Machine Learning and Data Mining</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -2293,16 +2293,16 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2329,11 +2329,11 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -2365,11 +2365,11 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -2401,16 +2401,16 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2421,11 +2421,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>571</v>
+        <v>199</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Advanced Machine Learning</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -2433,15 +2433,15 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>1:25-2:40pm</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -2457,11 +2457,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>523</v>
+        <v>571</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Advanced Machine Learning</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -2473,7 +2473,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2509,11 +2509,11 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -2529,11 +2529,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Focus </t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -2545,16 +2545,16 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2565,11 +2565,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>221</v>
+        <v>332</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Statistical Inference</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -2581,16 +2581,16 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2601,11 +2601,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>522</v>
+        <v>110</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Study Design</t>
+          <t xml:space="preserve">Focus </t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2613,20 +2613,20 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>Ugrad</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2637,11 +2637,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>702</v>
+        <v>522</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t>Study Design</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -2653,16 +2653,16 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
@@ -2763,7 +2763,7 @@
         <v>323</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -2772,12 +2772,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>11:45-1:00pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>M/W</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
@@ -2788,75 +2788,75 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>602</v>
+        <v>702</v>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Modern Data Analysis (grad students outside STATSCI)</t>
+          <t>Bayesian &amp; Modern</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>199</v>
+        <v>440</v>
       </c>
       <c r="C4" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Intro Data Science</t>
+          <t>Case Studies</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Predictive Modeling</t>
+          <t>Statistical Programming</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>10:05-11:20am</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2868,28 +2868,28 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>101</v>
+        <v>721</v>
       </c>
       <c r="C6" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Analy/Stat Inf </t>
+          <t>Linear Models</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6:15-7:30pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2900,24 +2900,24 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>410</v>
+        <v>221</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Hierarchical Models</t>
+          <t>Regression Analysis</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
@@ -2931,7 +2931,7 @@
         <v>610</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>8:30-9:45am</t>
+          <t>6:15-7:30pm</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2956,19 +2956,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>440</v>
+        <v>521</v>
       </c>
       <c r="C9" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Case Studies</t>
+          <t>Predictive Modeling</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1:25-2:40pm</t>
+          <t>8:30-9:45am</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2984,19 +2984,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>402</v>
+        <v>602</v>
       </c>
       <c r="C10" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern Statistics</t>
+          <t>Modern Data Analysis (grad students outside STATSCI)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -3012,14 +3012,14 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>721</v>
+        <v>410</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Linear Models</t>
+          <t>Hierarchical Models</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -3029,21 +3029,21 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>325</v>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -3052,30 +3052,30 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>4:40-5:55pm</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>W/F</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>198</v>
+        <v>402</v>
       </c>
       <c r="C13" t="n">
         <v>7</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Intro Health Data Science</t>
+          <t>Bayesian &amp; Modern Statistics</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -3092,74 +3092,74 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>240</v>
+        <v>198</v>
       </c>
       <c r="C14" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
+          <t>Intro Health Data Science</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3:05-4:20pm</t>
+          <t>11:45-1:00pm</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>T/TH</t>
+          <t>M/F</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>O</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>523</v>
+        <v>240</v>
       </c>
       <c r="C15" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Statistical Programming</t>
+          <t>Probability for Stat Inference, Modeling, &amp; Data Analysis</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>10:05-11:20am</t>
+          <t>3:05-4:20pm</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>M/F</t>
+          <t>M/W</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Regression Analysis</t>
+          <t>Intro Data Science</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -3169,25 +3169,25 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>W/F</t>
+          <t>T/TH</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>702</v>
+        <v>101</v>
       </c>
       <c r="C17" t="n">
         <v>11</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Bayesian &amp; Modern</t>
+          <t xml:space="preserve">Data Analy/Stat Inf </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">

</xml_diff>